<commit_message>
Start of the database remodel
</commit_message>
<xml_diff>
--- a/Rascunho DB.xlsx
+++ b/Rascunho DB.xlsx
@@ -8,13 +8,20 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="status" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="situacao" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="marketing" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="cursos" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="atendente" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="polos" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="candidatos" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="tipo" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="status_cand" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="status_insc" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="status_ex" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">candidatos!$A$1:$O$3</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -25,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t xml:space="preserve">Não atendeu</t>
   </si>
@@ -132,7 +139,19 @@
     <t xml:space="preserve">MARKETING</t>
   </si>
   <si>
-    <t xml:space="preserve">STATUS</t>
+    <t xml:space="preserve">TIPO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUS CAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUS_INSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUS_EX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SITUAÇÃO ATEND.</t>
   </si>
   <si>
     <t xml:space="preserve">ATENDENTE</t>
@@ -142,17 +161,66 @@
   </si>
   <si>
     <t xml:space="preserve">OBSERVAÇÕES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Candidato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsdnlnlksdfnvkldsvnl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joaquim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ex aluno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancelado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inscrito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Novo candidato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convocado Calouro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pré insc. Calouro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pré insc. port. diploma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pré inscrito transf. externa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abandono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concluído</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trancado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-----------</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -179,6 +247,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,7 +296,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,6 +309,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -246,6 +331,10 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -321,6 +410,58 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:A6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -538,25 +679,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="3" style="1" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="1" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="37.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="16" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,153 +738,230 @@
       <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J2" s="2"/>
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>44650</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J5" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J6" s="2"/>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J7" s="2"/>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J8" s="2"/>
+      <c r="N8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J9" s="2"/>
+      <c r="N9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J10" s="2"/>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="2"/>
+      <c r="N11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J12" s="2"/>
+      <c r="N12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J13" s="2"/>
+      <c r="N13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="2"/>
+      <c r="N14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="2"/>
+      <c r="N15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="2"/>
+      <c r="N16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J17" s="2"/>
+      <c r="N17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="2"/>
+      <c r="N18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J19" s="2"/>
+      <c r="N19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J20" s="2"/>
+      <c r="N20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J21" s="2"/>
+      <c r="N21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="2"/>
+      <c r="N22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="2"/>
+      <c r="N23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="2"/>
+      <c r="N24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J25" s="2"/>
+      <c r="N25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J26" s="2"/>
+      <c r="N26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J27" s="2"/>
+      <c r="N27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J28" s="2"/>
+      <c r="N28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="2"/>
+      <c r="N29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J30" s="2"/>
+      <c r="N30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="2"/>
+      <c r="N31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="2"/>
+      <c r="N32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J33" s="2"/>
+      <c r="N33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="2"/>
+      <c r="N34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="2"/>
+      <c r="N35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J36" s="2"/>
+      <c r="N36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J37" s="2"/>
+      <c r="N37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J38" s="2"/>
+      <c r="N38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="2"/>
+      <c r="N39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="2"/>
+      <c r="N40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J41" s="2"/>
+      <c r="N41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J42" s="2"/>
+      <c r="N42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J43" s="2"/>
+      <c r="N43" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <autoFilter ref="A1:O3"/>
+  <dataValidations count="10">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F43" type="list">
       <formula1>cursos!$A$1:$A$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G43" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 G4:G38 G39:K43" type="list">
       <formula1>marketing!$A$1:$A$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H43" type="list">
-      <formula1>status!$A$1:$A$10</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L43" type="list">
+      <formula1>situacao!$A$1:$A$10</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I43" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2:M43" type="list">
       <formula1>atendente!$A$1:$A$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A43" type="list">
       <formula1>polos!$A$1:$A$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H38" type="list">
+      <formula1>tipo!$A$1:$A$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I38" type="list">
+      <formula1>status_cand!$A$1:$A$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J38" type="list">
+      <formula1>status_insc!$A$1:$A$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K2:K38" type="list">
+      <formula1>status_ex!$A$1:$A$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G3" type="list">
+      <formula1>status_ex!$A$1:$A$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -750,5 +972,129 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:A4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:A5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>